<commit_message>
add arquivos, funçoes novas , corrigido e vericado
</commit_message>
<xml_diff>
--- a/Teste_Projeto.xlsx
+++ b/Teste_Projeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel\Desktop\Algoritimos em C\projeto-CCF110\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46A1F5D5-0909-4215-A5E1-7F2FA595CAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D04D2FE-9B97-43B2-A614-4071FEE2592F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{8486BDA4-B6C5-4D2F-9A08-20C55648BC67}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>WINS</t>
   </si>
@@ -102,13 +102,16 @@
   </si>
   <si>
     <t xml:space="preserve">Jogador </t>
+  </si>
+  <si>
+    <t>SE  QUISER  VERIFICAR OUTRAS COMPRAÇOES  DE MMRs DEVE ALTERAR NO ARQUIVO (SE QUISER CONFERIR A FUCIONALIDADE DO CODIGO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +121,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,18 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -302,48 +301,78 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,29 +380,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB1E7A0-BBE1-4094-A6C4-6F468CA20ACC}">
   <dimension ref="A2:AC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18:Q18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,222 +949,245 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I8" s="4" t="s">
+    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="I8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I9" s="17" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="I9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="17" t="s">
+      <c r="J9" s="17"/>
+      <c r="K9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="17" t="s">
+      <c r="L9" s="17"/>
+      <c r="M9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="11" t="s">
+      <c r="N9" s="17"/>
+      <c r="O9" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="12"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="27"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="16" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
+      <c r="Q10" s="24"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I11" s="5" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="I11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="13">
+      <c r="J11" s="21"/>
+      <c r="K11" s="22">
         <v>20</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="13">
+      <c r="L11" s="23"/>
+      <c r="M11" s="22">
         <v>0</v>
       </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="21">
+      <c r="N11" s="23"/>
+      <c r="O11" s="8">
         <v>200</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="26"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="32">
+      <c r="J12" s="36"/>
+      <c r="K12" s="28">
         <v>19</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="32">
+      <c r="L12" s="29"/>
+      <c r="M12" s="28">
         <v>1</v>
       </c>
-      <c r="N12" s="33"/>
-      <c r="O12" s="36">
+      <c r="N12" s="29"/>
+      <c r="O12" s="13">
         <v>180</v>
       </c>
-      <c r="P12" s="22" t="s">
+      <c r="P12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
-      <c r="AC12" s="26"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H13">
         <v>2</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="32">
+      <c r="J13" s="36"/>
+      <c r="K13" s="28">
         <v>18</v>
       </c>
-      <c r="L13" s="33"/>
-      <c r="M13" s="32">
+      <c r="L13" s="29"/>
+      <c r="M13" s="28">
         <v>2</v>
       </c>
-      <c r="N13" s="33"/>
-      <c r="O13" s="36">
+      <c r="N13" s="29"/>
+      <c r="O13" s="13">
         <v>160</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="P13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="Y13" s="26"/>
-      <c r="Z13" s="26"/>
-      <c r="AA13" s="26"/>
-      <c r="AB13" s="26"/>
-      <c r="AC13" s="26"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="13">
+      <c r="J14" s="21"/>
+      <c r="K14" s="22">
         <v>17</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="13">
+      <c r="L14" s="23"/>
+      <c r="M14" s="22">
         <v>3</v>
       </c>
-      <c r="N14" s="14"/>
-      <c r="O14" s="23">
+      <c r="N14" s="23"/>
+      <c r="O14" s="9">
         <v>140</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="P14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="13">
+      <c r="J15" s="21"/>
+      <c r="K15" s="22">
         <v>16</v>
       </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="13">
+      <c r="L15" s="23"/>
+      <c r="M15" s="22">
         <v>4</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="23">
+      <c r="N15" s="23"/>
+      <c r="O15" s="9">
         <v>120</v>
       </c>
-      <c r="P15" s="22" t="s">
+      <c r="P15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="Y15" s="26"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="37"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H16">
         <v>3</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="28"/>
+      <c r="J16" s="34"/>
       <c r="K16" s="30">
         <v>15</v>
       </c>
@@ -1158,223 +1196,197 @@
         <v>5</v>
       </c>
       <c r="N16" s="31"/>
-      <c r="O16" s="29">
+      <c r="O16" s="12">
         <v>100</v>
       </c>
-      <c r="P16" s="22" t="s">
+      <c r="P16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
     </row>
     <row r="17" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="13">
+      <c r="J17" s="21"/>
+      <c r="K17" s="22">
         <v>14</v>
       </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="13">
+      <c r="L17" s="23"/>
+      <c r="M17" s="22">
         <v>6</v>
       </c>
-      <c r="N17" s="14"/>
-      <c r="O17" s="23">
+      <c r="N17" s="23"/>
+      <c r="O17" s="9">
         <v>80</v>
       </c>
-      <c r="P17" s="22" t="s">
+      <c r="P17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="26"/>
-      <c r="AC17" s="26"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
     </row>
     <row r="18" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="13">
+      <c r="J18" s="21"/>
+      <c r="K18" s="22">
         <v>13</v>
       </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="13">
+      <c r="L18" s="23"/>
+      <c r="M18" s="22">
         <v>7</v>
       </c>
-      <c r="N18" s="14"/>
-      <c r="O18" s="23">
+      <c r="N18" s="23"/>
+      <c r="O18" s="9">
         <v>60</v>
       </c>
-      <c r="P18" s="22" t="s">
+      <c r="P18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
     </row>
     <row r="19" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="13">
+      <c r="J19" s="21"/>
+      <c r="K19" s="22">
         <v>12</v>
       </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="13">
+      <c r="L19" s="23"/>
+      <c r="M19" s="22">
         <v>8</v>
       </c>
-      <c r="N19" s="14"/>
-      <c r="O19" s="23">
+      <c r="N19" s="23"/>
+      <c r="O19" s="9">
         <v>40</v>
       </c>
-      <c r="P19" s="22" t="s">
+      <c r="P19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="26"/>
-      <c r="AC19" s="26"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
     </row>
     <row r="20" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="13">
+      <c r="J20" s="21"/>
+      <c r="K20" s="22">
         <v>11</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="13">
+      <c r="L20" s="23"/>
+      <c r="M20" s="22">
         <v>9</v>
       </c>
-      <c r="N20" s="14"/>
-      <c r="O20" s="23">
+      <c r="N20" s="23"/>
+      <c r="O20" s="9">
         <v>20</v>
       </c>
-      <c r="P20" s="22" t="s">
+      <c r="P20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="Y20" s="25"/>
-      <c r="Z20" s="25"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="25"/>
-      <c r="AC20" s="25"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
     </row>
     <row r="21" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="13">
+      <c r="J21" s="21"/>
+      <c r="K21" s="22">
         <v>10</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="13">
+      <c r="L21" s="23"/>
+      <c r="M21" s="22">
         <v>10</v>
       </c>
-      <c r="N21" s="14"/>
-      <c r="O21" s="23">
+      <c r="N21" s="23"/>
+      <c r="O21" s="9">
         <v>0</v>
       </c>
-      <c r="P21" s="22" t="s">
+      <c r="P21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="Q21" s="22"/>
+      <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
     </row>
     <row r="23" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
+  <mergeCells count="56">
+    <mergeCell ref="C8:F12"/>
+    <mergeCell ref="I8:Q8"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
@@ -1389,15 +1401,43 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I8:Q8"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>